<commit_message>
MA0901: Ajustes de esqueleto y archivo de segProdDigital
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion01/EsqueletoGuion_MA_09_01_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion01/EsqueletoGuion_MA_09_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado09\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado09\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="7230" tabRatio="729" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="7230" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="77">
   <si>
     <t>FICHA</t>
   </si>
@@ -192,34 +192,7 @@
     <t>sí</t>
   </si>
   <si>
-    <t>Comprende el conjunto de los números reales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prueba tus conocimientos del conjunto de los números reales </t>
-  </si>
-  <si>
-    <r>
-      <t>Aproximación de números reales; el precio por aproximarlos es el error</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Calcula el error absoluto y el error relativo </t>
-  </si>
-  <si>
-    <t>Los intervalos y tipos de intervalos en la recta real</t>
-  </si>
-  <si>
-    <t>Practica la representación de intervalos en la recta real</t>
   </si>
   <si>
     <t xml:space="preserve">Los conjuntos numéricos </t>
@@ -295,7 +268,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,13 +332,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1622,17 +1588,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="2" max="2" width="104.265625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
@@ -1640,7 +1606,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
@@ -1648,7 +1614,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
@@ -1656,7 +1622,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
@@ -1664,7 +1630,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1672,7 +1638,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
@@ -1699,19 +1665,19 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.73046875" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -1731,7 +1697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="16" t="s">
         <v>21</v>
       </c>
@@ -1757,7 +1723,7 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="16" t="s">
         <v>21</v>
       </c>
@@ -1777,7 +1743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="16" t="s">
         <v>21</v>
       </c>
@@ -1797,7 +1763,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="16" t="s">
         <v>21</v>
       </c>
@@ -1817,7 +1783,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="16" t="s">
         <v>21</v>
       </c>
@@ -1837,7 +1803,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
         <v>21</v>
       </c>
@@ -1857,20 +1823,20 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="F9" s="4"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G12" s="7"/>
     </row>
   </sheetData>
@@ -1889,16 +1855,16 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C2" sqref="C2:C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="66.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="66.1328125" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -1909,7 +1875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>33</v>
       </c>
@@ -1920,7 +1886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>35</v>
       </c>
@@ -1931,7 +1897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>36</v>
       </c>
@@ -1942,7 +1908,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="19" t="s">
         <v>37</v>
       </c>
@@ -1953,7 +1919,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="19" t="s">
         <v>38</v>
       </c>
@@ -1964,7 +1930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="19" t="s">
         <v>39</v>
       </c>
@@ -1975,7 +1941,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="19" t="s">
         <v>40</v>
       </c>
@@ -1986,7 +1952,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="19" t="s">
         <v>42</v>
       </c>
@@ -1997,7 +1963,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="19" t="s">
         <v>41</v>
       </c>
@@ -2008,7 +1974,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="19" t="s">
         <v>43</v>
       </c>
@@ -2019,7 +1985,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="19" t="s">
         <v>44</v>
       </c>
@@ -2030,7 +1996,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="19" t="s">
         <v>45</v>
       </c>
@@ -2041,7 +2007,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="19" t="s">
         <v>46</v>
       </c>
@@ -2052,7 +2018,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="19" t="s">
         <v>47</v>
       </c>
@@ -2063,7 +2029,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A16" s="19" t="s">
         <v>48</v>
       </c>
@@ -2074,7 +2040,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="19" t="s">
         <v>49</v>
       </c>
@@ -2085,7 +2051,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="19" t="s">
         <v>50</v>
       </c>
@@ -2096,7 +2062,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="19" t="s">
         <v>51</v>
       </c>
@@ -2107,42 +2073,42 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="17"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="17"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="17"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="17"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="17"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
@@ -2168,18 +2134,18 @@
   </sheetPr>
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:C33"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="92.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.265625" customWidth="1"/>
+    <col min="3" max="3" width="19.265625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
@@ -2190,7 +2156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2201,7 +2167,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -2212,7 +2178,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -2223,7 +2189,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -2234,7 +2200,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -2245,7 +2211,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -2256,18 +2222,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -2278,40 +2244,40 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -2322,29 +2288,29 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -2355,7 +2321,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -2366,7 +2332,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -2377,7 +2343,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -2388,7 +2354,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -2399,7 +2365,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -2410,7 +2376,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -2421,7 +2387,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -2432,7 +2398,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -2443,7 +2409,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -2454,42 +2420,42 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="5"/>
       <c r="B26" s="19"/>
       <c r="C26"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="5"/>
       <c r="B27" s="19"/>
       <c r="C27"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="5"/>
       <c r="B28" s="19"/>
       <c r="C28"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="5"/>
       <c r="B29" s="19"/>
       <c r="C29"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="5"/>
       <c r="B30" s="19"/>
       <c r="C30"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="5"/>
       <c r="B31" s="19"/>
       <c r="C31"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="5"/>
       <c r="B32" s="19"/>
       <c r="C32"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="5"/>
       <c r="B33" s="19"/>
       <c r="C33"/>
@@ -2513,24 +2479,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView topLeftCell="E17" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="46.85546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.86328125" customWidth="1"/>
+    <col min="2" max="2" width="42.1328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="51.265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.86328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="46.86328125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.86328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="64.1328125" customWidth="1"/>
+    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -2559,15 +2525,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D2" s="30"/>
       <c r="E2" s="30"/>
@@ -2576,15 +2542,15 @@
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
@@ -2593,15 +2559,15 @@
       <c r="H3" s="30"/>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D4" s="30"/>
       <c r="E4" s="30"/>
@@ -2610,15 +2576,15 @@
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D5" s="30"/>
       <c r="E5" s="15"/>
@@ -2627,15 +2593,15 @@
       <c r="H5" s="13"/>
       <c r="I5" s="30"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="15"/>
@@ -2648,114 +2614,114 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C7" s="23"/>
       <c r="D7" s="23" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F7" s="24"/>
       <c r="G7" s="24"/>
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="23" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="24"/>
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="23" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="24"/>
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="23" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="24"/>
       <c r="H10" s="22"/>
       <c r="I10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="23" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="24"/>
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="23" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="24"/>
@@ -2766,19 +2732,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="23" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F13" s="24"/>
       <c r="G13" s="24"/>
@@ -2789,19 +2755,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="23" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
@@ -2812,95 +2778,95 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="23" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
       <c r="H15" s="22"/>
       <c r="I15" s="20"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="23" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
       <c r="H16" s="22"/>
       <c r="I16" s="20"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="23" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F17" s="20"/>
       <c r="G17" s="20"/>
       <c r="H17" s="22"/>
       <c r="I17" s="20"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="23" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
       <c r="H18" s="22"/>
       <c r="I18" s="20"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="23" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F19" s="20"/>
       <c r="G19" s="20"/>
@@ -2911,19 +2877,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="23" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
@@ -2934,76 +2900,76 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="31" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F21" s="29"/>
       <c r="G21" s="29"/>
       <c r="H21" s="13"/>
       <c r="I21" s="29"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C22" s="29"/>
       <c r="D22" s="31" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F22" s="29"/>
       <c r="G22" s="29"/>
       <c r="H22" s="29"/>
       <c r="I22" s="29"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C23" s="29"/>
       <c r="D23" s="31" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F23" s="29"/>
       <c r="G23" s="29"/>
       <c r="H23" s="29"/>
       <c r="I23" s="29"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C24" s="29"/>
       <c r="D24" s="31" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F24" s="29"/>
       <c r="G24" s="29"/>
@@ -3014,19 +2980,19 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C25" s="29"/>
       <c r="D25" s="31" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F25" s="29"/>
       <c r="G25" s="29"/>
@@ -3037,19 +3003,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C26" s="29"/>
       <c r="D26" s="31" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F26" s="29"/>
       <c r="G26" s="29"/>
@@ -3060,44 +3026,44 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C27" s="29"/>
       <c r="D27" s="31" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E27" s="29"/>
       <c r="F27" s="32" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G27" s="29" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H27" s="29"/>
       <c r="I27" s="29"/>
     </row>
-    <row r="28" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C28" s="29"/>
       <c r="D28" s="31" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E28" s="29"/>
       <c r="F28" s="32" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G28" s="33" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H28" s="16" t="s">
         <v>26</v>
@@ -3106,23 +3072,23 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C29" s="29"/>
       <c r="D29" s="31" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E29" s="34"/>
       <c r="F29" s="32" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G29" s="29" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H29" s="16" t="s">
         <v>27</v>
@@ -3131,38 +3097,38 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C30" s="36"/>
       <c r="D30" s="36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E30" s="36" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
       <c r="H30" s="36"/>
       <c r="I30" s="36"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B31" s="35" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C31" s="36"/>
       <c r="D31" s="36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E31" s="36" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F31" s="36"/>
       <c r="G31" s="36"/>
@@ -3173,271 +3139,271 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B32" s="35" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C32" s="36"/>
       <c r="D32" s="36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E32" s="36" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F32" s="36"/>
       <c r="G32" s="36"/>
       <c r="H32" s="36"/>
       <c r="I32" s="36"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B33" s="35" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C33" s="36"/>
       <c r="D33" s="36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E33" s="36" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F33" s="36"/>
       <c r="G33" s="36"/>
       <c r="H33" s="36"/>
       <c r="I33" s="36"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B34" s="35" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C34" s="36"/>
       <c r="D34" s="36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E34" s="36"/>
       <c r="F34" s="39" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G34" s="36" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H34" s="36"/>
       <c r="I34" s="36"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B35" s="35" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C35" s="36"/>
       <c r="D35" s="36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E35" s="36"/>
       <c r="F35" s="39" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G35" s="36" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H35" s="36"/>
       <c r="I35" s="36"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B36" s="35" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C36" s="36"/>
       <c r="D36" s="36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E36" s="36"/>
       <c r="F36" s="39" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G36" s="36" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H36" s="36"/>
       <c r="I36" s="36"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B37" s="35" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C37" s="36"/>
       <c r="D37" s="36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E37" s="36"/>
       <c r="F37" s="39" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G37" s="36" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H37" s="36"/>
       <c r="I37" s="36"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B38" s="35" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C38" s="36"/>
       <c r="D38" s="36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E38" s="36"/>
       <c r="F38" s="39" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G38" s="36" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H38" s="36"/>
       <c r="I38" s="36"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B39" s="35" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C39" s="36"/>
       <c r="D39" s="36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E39" s="36"/>
       <c r="F39" s="39" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G39" s="36" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H39" s="40"/>
       <c r="I39" s="36"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B40" s="35" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C40" s="36"/>
       <c r="D40" s="36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E40" s="36"/>
       <c r="F40" s="39" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G40" s="36" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H40" s="36"/>
       <c r="I40" s="36"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B41" s="35" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C41" s="36"/>
       <c r="D41" s="36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E41" s="36"/>
       <c r="F41" s="39" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G41" s="36" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H41" s="40"/>
       <c r="I41" s="36"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B42" s="35" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C42" s="38"/>
       <c r="D42" s="36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E42" s="38"/>
       <c r="F42" s="39" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G42" s="36" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H42" s="36"/>
       <c r="I42" s="38"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B43" s="35" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C43" s="38"/>
       <c r="D43" s="36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E43" s="38"/>
       <c r="F43" s="39" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G43" s="36" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H43" s="40"/>
       <c r="I43" s="38"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B44" s="35" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C44" s="38"/>
       <c r="D44" s="36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E44" s="38"/>
       <c r="F44" s="39" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G44" s="38" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H44" s="16" t="s">
         <v>28</v>
@@ -3446,23 +3412,23 @@
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B45" s="35" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C45" s="38"/>
       <c r="D45" s="36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E45" s="38"/>
       <c r="F45" s="39" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G45" s="38" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H45" s="16" t="s">
         <v>29</v>
@@ -3471,23 +3437,23 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B46" s="35" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C46" s="38"/>
       <c r="D46" s="36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E46" s="38"/>
       <c r="F46" s="39" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G46" s="38" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H46" s="37" t="s">
         <v>41</v>
@@ -3496,38 +3462,38 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B47" s="30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C47" s="13"/>
       <c r="D47" s="29" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B48" s="30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C48" s="13"/>
       <c r="D48" s="29" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
@@ -3538,15 +3504,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="22"/>
@@ -3555,15 +3521,15 @@
       <c r="H49" s="25"/>
       <c r="I49" s="22"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D50" s="20"/>
       <c r="E50" s="22"/>
@@ -3572,15 +3538,15 @@
       <c r="H50" s="25"/>
       <c r="I50" s="22"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="22"/>
@@ -3589,15 +3555,15 @@
       <c r="H51" s="25"/>
       <c r="I51" s="22"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
@@ -3606,152 +3572,152 @@
       <c r="H52" s="22"/>
       <c r="I52" s="22"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C53" s="22"/>
       <c r="D53" s="20" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F53" s="22"/>
       <c r="G53" s="22"/>
       <c r="H53" s="22"/>
       <c r="I53" s="22"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C54" s="22"/>
       <c r="D54" s="20" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F54" s="22"/>
       <c r="G54" s="22"/>
       <c r="H54" s="22"/>
       <c r="I54" s="22"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C55" s="22"/>
       <c r="D55" s="20" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E55" s="22" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F55" s="22"/>
       <c r="G55" s="22"/>
       <c r="H55" s="22"/>
       <c r="I55" s="22"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B56" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C56" s="22"/>
       <c r="D56" s="20" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E56" s="22" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F56" s="26"/>
       <c r="G56" s="22"/>
       <c r="H56" s="22"/>
       <c r="I56" s="22"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B57" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C57" s="22"/>
       <c r="D57" s="20" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E57" s="22" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F57" s="26"/>
       <c r="G57" s="26"/>
       <c r="H57" s="26"/>
       <c r="I57" s="22"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C58" s="22"/>
       <c r="D58" s="20" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F58" s="26"/>
       <c r="G58" s="26"/>
       <c r="H58" s="26"/>
       <c r="I58" s="22"/>
     </row>
-    <row r="59" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C59" s="27"/>
       <c r="D59" s="20" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E59" s="27" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F59" s="24"/>
       <c r="G59" s="26"/>
       <c r="H59" s="26"/>
       <c r="I59" s="27"/>
     </row>
-    <row r="60" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B60" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C60" s="22"/>
       <c r="D60" s="20" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E60" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F60" s="22"/>
       <c r="G60" s="26"/>
@@ -3762,19 +3728,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B61" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C61" s="22"/>
       <c r="D61" s="20" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E61" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F61" s="22"/>
       <c r="G61" s="26"/>
@@ -3785,19 +3751,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C62" s="22"/>
       <c r="D62" s="20" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E62" s="20" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F62" s="20"/>
       <c r="G62" s="20"/>
@@ -3808,19 +3774,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B63" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C63" s="22"/>
       <c r="D63" s="20" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E63" s="20" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F63" s="20"/>
       <c r="G63" s="20"/>
@@ -3831,38 +3797,38 @@
         <v>19</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C64" s="22"/>
       <c r="D64" s="25" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E64" s="20" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F64" s="20"/>
       <c r="G64" s="20"/>
       <c r="H64" s="26"/>
       <c r="I64" s="22"/>
     </row>
-    <row r="65" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C65" s="22"/>
       <c r="D65" s="25" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E65" s="20" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F65" s="20"/>
       <c r="G65" s="20"/>
@@ -3873,15 +3839,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C66" s="38" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D66" s="38"/>
       <c r="E66" s="38"/>
@@ -3890,15 +3856,15 @@
       <c r="H66" s="37"/>
       <c r="I66" s="38"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B67" s="37" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C67" s="38" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D67" s="38"/>
       <c r="E67" s="38"/>
@@ -3911,15 +3877,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B68" s="37" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C68" s="38" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D68" s="38"/>
       <c r="E68" s="38"/>
@@ -3930,15 +3896,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B69" s="36" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C69" s="36" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D69" s="36"/>
       <c r="E69" s="36"/>
@@ -3949,7 +3915,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" s="20"/>
       <c r="B70" s="20"/>
       <c r="C70" s="20"/>
@@ -3960,7 +3926,7 @@
       <c r="H70" s="26"/>
       <c r="I70" s="22"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" s="20"/>
       <c r="B71" s="20"/>
       <c r="C71" s="20"/>
@@ -3971,7 +3937,7 @@
       <c r="H71" s="26"/>
       <c r="I71" s="22"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" s="20"/>
       <c r="B72" s="28"/>
       <c r="C72" s="28"/>
@@ -3982,7 +3948,7 @@
       <c r="H72" s="28"/>
       <c r="I72" s="28"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" s="20"/>
       <c r="B73" s="28"/>
       <c r="C73" s="28"/>

</xml_diff>